<commit_message>
Fixed issues with chromedriver with OS and updated documentation
</commit_message>
<xml_diff>
--- a/converted-currency.xlsx
+++ b/converted-currency.xlsx
@@ -24,10 +24,10 @@
     <t>Converted Value</t>
   </si>
   <si>
-    <t>33.11</t>
+    <t>93.29</t>
   </si>
   <si>
-    <t>27.30</t>
+    <t>76.92</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Fixed rounding issues and added more prints
</commit_message>
<xml_diff>
--- a/converted-currency.xlsx
+++ b/converted-currency.xlsx
@@ -24,10 +24,10 @@
     <t>Converted Value</t>
   </si>
   <si>
-    <t>93.29</t>
+    <t>71.31</t>
   </si>
   <si>
-    <t>76.92</t>
+    <t>58.80</t>
   </si>
 </sst>
 </file>

</xml_diff>